<commit_message>
feat：update skill icon excel
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionSkill_技能表.xlsx
+++ b/battleworld/Excel/MotionSkill_技能表.xlsx
@@ -1834,11 +1834,11 @@
   <dimension ref="A1:X84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+      <selection pane="bottomRight" activeCell="E64" activeCellId="0" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>